<commit_message>
Mostly implemented channel tests.  Just need to figure out an easy way to add participants manually.  Added abstract event and individual and group tests will implement soon.  Still adding to excel file spreadsheat.
</commit_message>
<xml_diff>
--- a/required_project_files/Test Cases.xlsx
+++ b/required_project_files/Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13920" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Black Box Test" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
   <si>
     <t>Test Id</t>
   </si>
@@ -305,13 +305,22 @@
     <t>The event id is returned</t>
   </si>
   <si>
-    <t>Create new channel</t>
-  </si>
-  <si>
-    <t>Create channel with specified sensor type</t>
-  </si>
-  <si>
-    <t>Create channel with a sensor type that does not exist</t>
+    <t>Create new channel with default system controller, valid id and null sensor</t>
+  </si>
+  <si>
+    <t>Create new channel with default system controller, valid id and invalid sensor name</t>
+  </si>
+  <si>
+    <t>Create new channel with default system controller, valid id and valid sensor name</t>
+  </si>
+  <si>
+    <t>Channel constructor throws Illegal Argument exception</t>
+  </si>
+  <si>
+    <t>Channel is created without exception but with no active sensor</t>
+  </si>
+  <si>
+    <t>Channel is created without exception and with an active sensor type</t>
   </si>
 </sst>
 </file>
@@ -762,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="BS1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1518,14 +1527,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1549,6 +1558,9 @@
       <c r="B2" t="s">
         <v>93</v>
       </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
@@ -1557,6 +1569,9 @@
       <c r="B3" t="s">
         <v>94</v>
       </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
@@ -1566,7 +1581,7 @@
         <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>

<commit_message>
Updated excel sheet and removed old abstract event test
</commit_message>
<xml_diff>
--- a/required_project_files/Test Cases.xlsx
+++ b/required_project_files/Test Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
   <si>
     <t>Test Id</t>
   </si>
@@ -321,6 +321,93 @@
   </si>
   <si>
     <t>Channel is created without exception and with an active sensor type</t>
+  </si>
+  <si>
+    <t>Create new channel with default system controller, valid id, valid sensor name and not active</t>
+  </si>
+  <si>
+    <t>Create new channel with default system controller, valid id, valid sensor name and is active</t>
+  </si>
+  <si>
+    <t>Add sensor to the channel with string of "GATE"</t>
+  </si>
+  <si>
+    <t>Add sensor to channel with string of "bad sensor"</t>
+  </si>
+  <si>
+    <t>Illegal argument Exception for trying to add an invalid sensor type</t>
+  </si>
+  <si>
+    <t>Channel adds a sensor of type gate</t>
+  </si>
+  <si>
+    <t>Add a sensor to the channel with a sensor of type PAD</t>
+  </si>
+  <si>
+    <t>Channel's sensor is set to a PAD</t>
+  </si>
+  <si>
+    <t>Same as expected</t>
+  </si>
+  <si>
+    <t>Same as expedted</t>
+  </si>
+  <si>
+    <t>Channel is created and is not active(false)</t>
+  </si>
+  <si>
+    <t>Channel is created and is active(true)</t>
+  </si>
+  <si>
+    <t>same as expected</t>
+  </si>
+  <si>
+    <t>A channel with sensor of type PAD has sensor disconnected</t>
+  </si>
+  <si>
+    <t>Channel's sensor is null and sensor type is null</t>
+  </si>
+  <si>
+    <t>Trigger channel's sensor that is not active(false)</t>
+  </si>
+  <si>
+    <t>The sensor is not triggered because channel is not active</t>
+  </si>
+  <si>
+    <t>Trigger a channel's sensor that is active(true) but sensor is null</t>
+  </si>
+  <si>
+    <t>the sensor is not triggered because it does not exist</t>
+  </si>
+  <si>
+    <t>Test get channel state when not active</t>
+  </si>
+  <si>
+    <t>The state is not active so false</t>
+  </si>
+  <si>
+    <t>test get channel state when active</t>
+  </si>
+  <si>
+    <t>The state is true because it is active</t>
+  </si>
+  <si>
+    <t>Get channel id with id 0f 100</t>
+  </si>
+  <si>
+    <t>id is returned to be 100</t>
+  </si>
+  <si>
+    <t>Channel exit</t>
+  </si>
+  <si>
+    <t>Id is -1, active is false and current sensor is set to null if there was on</t>
+  </si>
+  <si>
+    <t>Channel trigger sensor no sensor</t>
+  </si>
+  <si>
+    <t>cannot trigger sensor since nul</t>
   </si>
 </sst>
 </file>
@@ -1525,16 +1612,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="69.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1561,6 +1649,9 @@
       <c r="C2" t="s">
         <v>97</v>
       </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
@@ -1572,6 +1663,9 @@
       <c r="C3" t="s">
         <v>96</v>
       </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
@@ -1583,10 +1677,200 @@
       <c r="C4" t="s">
         <v>98</v>
       </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished test but some paper work is a little sparce.  We'll be ok.
</commit_message>
<xml_diff>
--- a/required_project_files/Test Cases.xlsx
+++ b/required_project_files/Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13920" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Black Box Test" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="165">
   <si>
     <t>Test Id</t>
   </si>
@@ -62,24 +62,9 @@
     <t>A participant starting but canceling the start due to invalid start</t>
   </si>
   <si>
-    <t>Turning the chrono timer system on</t>
-  </si>
-  <si>
-    <t>Turning the chrono timer system off</t>
-  </si>
-  <si>
-    <t>Exiting the chrono timer</t>
-  </si>
-  <si>
-    <t>Set the time</t>
-  </si>
-  <si>
     <t>Reset the timer</t>
   </si>
   <si>
-    <t>Toggle a channel</t>
-  </si>
-  <si>
     <t>Export event and participant data</t>
   </si>
   <si>
@@ -408,6 +393,132 @@
   </si>
   <si>
     <t>cannot trigger sensor since nul</t>
+  </si>
+  <si>
+    <t>Turning the chrono timer system on when starting up</t>
+  </si>
+  <si>
+    <t>Turning the chrono timer system off when already on</t>
+  </si>
+  <si>
+    <t>Exiting the chrono timer when on</t>
+  </si>
+  <si>
+    <t>Set the time on initialization</t>
+  </si>
+  <si>
+    <t>Toggle a channel on and off (enabled/disabled)</t>
+  </si>
+  <si>
+    <t>Run an Indivdiual event with 3 participants</t>
+  </si>
+  <si>
+    <t>Run a Group event with 2 participants</t>
+  </si>
+  <si>
+    <t>Run Test data from d2l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The chrono timer is initialized </t>
+  </si>
+  <si>
+    <t>The timer is turned off but</t>
+  </si>
+  <si>
+    <t>Set abstract event name to "new name"</t>
+  </si>
+  <si>
+    <t>the name is "new name"</t>
+  </si>
+  <si>
+    <t>Set event name to ""</t>
+  </si>
+  <si>
+    <t>The name is ""</t>
+  </si>
+  <si>
+    <t>Set event time to time.getTime()</t>
+  </si>
+  <si>
+    <t>The time is time.getTime()</t>
+  </si>
+  <si>
+    <t>Input invalid trig command format on GUI "Trig 55" invalid channel</t>
+  </si>
+  <si>
+    <t>Input invalid command "ON 294"</t>
+  </si>
+  <si>
+    <t>Add null participant to event</t>
+  </si>
+  <si>
+    <t>IllegalArgumentexception</t>
+  </si>
+  <si>
+    <t>Add participant already in current participants for event</t>
+  </si>
+  <si>
+    <t>Illegal Argument Exception</t>
+  </si>
+  <si>
+    <t>Add participant not already in queue and not null</t>
+  </si>
+  <si>
+    <t>The participant is added to current participants and is placed in the starting queue</t>
+  </si>
+  <si>
+    <t>Reset event with 3 participants in event</t>
+  </si>
+  <si>
+    <t>The participants are still in the event because reset event is used for cancel</t>
+  </si>
+  <si>
+    <t>Get event type of individual</t>
+  </si>
+  <si>
+    <t>Get event type of group</t>
+  </si>
+  <si>
+    <t>The individual event type is returned</t>
+  </si>
+  <si>
+    <t>The group event type is returned</t>
+  </si>
+  <si>
+    <t>Get event name with name of "Some name"</t>
+  </si>
+  <si>
+    <t>"Some name" is returned</t>
+  </si>
+  <si>
+    <t>Exit event</t>
+  </si>
+  <si>
+    <t>Event has all participant data structures to null</t>
+  </si>
+  <si>
+    <t>The command is not executed</t>
+  </si>
+  <si>
+    <t>The command is not executed but exception is thrown (need to fix)</t>
+  </si>
+  <si>
+    <t>The command is not exicuted</t>
+  </si>
+  <si>
+    <t>Start participants right after starting up GUI</t>
+  </si>
+  <si>
+    <t>The command is not executed but console says "Starting participants"</t>
+  </si>
+  <si>
+    <t>Finish participants without starting or turning on system</t>
+  </si>
+  <si>
+    <t>The command is not executed and considered invaid</t>
+  </si>
+  <si>
+    <t>The command is not executed but the console says "Finishing participants"</t>
   </si>
 </sst>
 </file>
@@ -463,8 +574,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -498,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -513,6 +628,8 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -527,6 +644,8 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -856,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="BS1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -928,7 +1047,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -936,7 +1058,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -944,7 +1069,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -952,7 +1077,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -960,7 +1085,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -968,7 +1093,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -976,7 +1101,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -984,7 +1109,84 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1000,18 +1202,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1032,40 +1234,154 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1113,13 +1429,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1127,13 +1443,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1141,13 +1457,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1155,13 +1471,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1169,13 +1485,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1183,13 +1499,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1197,13 +1513,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1211,13 +1527,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1225,13 +1541,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1239,13 +1555,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1293,10 +1609,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -1305,10 +1621,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1317,10 +1633,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -1329,10 +1645,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1341,10 +1657,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1353,10 +1669,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -1365,10 +1681,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1377,10 +1693,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1389,10 +1705,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1440,10 +1756,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1451,10 +1767,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1462,10 +1778,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1473,10 +1789,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1484,10 +1800,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1495,10 +1811,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1506,10 +1822,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1517,10 +1833,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1528,10 +1844,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1539,10 +1855,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1550,10 +1866,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1561,10 +1877,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1572,10 +1888,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1583,10 +1899,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1594,10 +1910,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1614,7 +1930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B2" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1644,13 +1960,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1658,13 +1974,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1672,13 +1988,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1686,13 +2002,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1700,13 +2016,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1714,13 +2030,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
         <v>106</v>
-      </c>
-      <c r="D7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1728,13 +2044,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1742,13 +2058,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1756,13 +2072,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1770,13 +2086,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1784,13 +2100,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1798,13 +2114,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1812,13 +2128,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1826,13 +2142,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1840,13 +2156,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1854,13 +2170,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4">

</xml_diff>